<commit_message>
Exporting production files in progress
Creating production files. Missing: ECO, Stackup, Drill
</commit_message>
<xml_diff>
--- a/KW2CPU.PCB Production Files/KW2CPU.PCB.BOM.xlsx
+++ b/KW2CPU.PCB Production Files/KW2CPU.PCB.BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="141">
   <si>
     <t>Qty</t>
   </si>
@@ -203,6 +203,9 @@
     <t>J1</t>
   </si>
   <si>
+    <t>Hirose DF12 Male Connector</t>
+  </si>
+  <si>
     <t>Hirose</t>
   </si>
   <si>
@@ -215,6 +218,9 @@
     <t>J2</t>
   </si>
   <si>
+    <t>Flat programming connector</t>
+  </si>
+  <si>
     <t>MOLEX</t>
   </si>
   <si>
@@ -227,6 +233,9 @@
     <t>J3</t>
   </si>
   <si>
+    <t>MMCX Antenna Connector</t>
+  </si>
+  <si>
     <t>Molex</t>
   </si>
   <si>
@@ -365,6 +374,9 @@
     <t>U3</t>
   </si>
   <si>
+    <t>RF Front End (PA / LNA)</t>
+  </si>
+  <si>
     <t>RFMD</t>
   </si>
   <si>
@@ -399,6 +411,9 @@
   </si>
   <si>
     <t>X1</t>
+  </si>
+  <si>
+    <t>32Khz Crystal</t>
   </si>
   <si>
     <t>EPSON</t>
@@ -532,7 +547,7 @@
   <dimension ref="1:35"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -929,11 +944,14 @@
       <c r="E15" s="0" t="s">
         <v>61</v>
       </c>
+      <c r="F15" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="G15" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,22 +959,25 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>67</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,19 +985,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>72</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>734152061</v>
@@ -987,7 +1011,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>18</v>
@@ -996,16 +1020,16 @@
         <v>18</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,25 +1037,25 @@
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,25 +1063,25 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>24</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1068,22 +1092,22 @@
         <v>0</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>24</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,25 +1115,25 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>83</v>
-      </c>
       <c r="H22" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,25 +1141,25 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>83</v>
-      </c>
       <c r="H23" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,25 +1167,25 @@
         <v>2</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C24" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>83</v>
-      </c>
       <c r="H24" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1172,22 +1196,22 @@
         <v>0</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1195,25 +1219,25 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>24</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1224,22 +1248,22 @@
         <v>0</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>24</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1250,22 +1274,22 @@
         <v>0</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>24</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>34</v>
@@ -1276,19 +1300,19 @@
         <v>12</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I29" s="0" t="s">
         <v>34</v>
@@ -1299,25 +1323,25 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1325,22 +1349,25 @@
         <v>1</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>119</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1348,22 +1375,22 @@
         <v>1</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="G32" s="0" t="s">
         <v>58</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1371,19 +1398,19 @@
         <v>1</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="I33" s="0" t="s">
         <v>34</v>
@@ -1394,22 +1421,25 @@
         <v>1</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>132</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1417,25 +1447,25 @@
         <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>